<commit_message>
Further Eval of the survey. Agreement Distance and interpretability
</commit_message>
<xml_diff>
--- a/JanEngler/Praktikum/Survey/Rating Countries, Food and Music on an Antonym-Scale (Antworten).xlsx
+++ b/JanEngler/Praktikum/Survey/Rating Countries, Food and Music on an Antonym-Scale (Antworten).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Desktop\Uni\Corona\Semantic\Semantic-Differentials-for-Wikipedia-using-the-POLAR-Framework\JanEngler\Praktikum\Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE4BC6C-4B50-4659-B340-240F06192A9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5608394B-ABD6-489C-BC0B-D9F70B9DE49E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formularantworten 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="143">
   <si>
     <t>Zeitstempel</t>
   </si>
@@ -464,6 +464,24 @@
   </si>
   <si>
     <t>-3.0293212 -2.3457592  2.047324   2.047324   1.9114097</t>
+  </si>
+  <si>
+    <t>Mean of stds</t>
+  </si>
+  <si>
+    <t>Countriy</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Reg:</t>
+  </si>
+  <si>
+    <t>Ext:</t>
   </si>
 </sst>
 </file>
@@ -748,11 +766,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BN51"/>
+  <dimension ref="A1:BN55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AW51" sqref="AW51"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -760,7 +778,7 @@
     <col min="1" max="72" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +978,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44013.51978707176</v>
       </c>
@@ -1151,7 +1169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44013.520650474537</v>
       </c>
@@ -1351,7 +1369,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44013.523335138889</v>
       </c>
@@ -1542,7 +1560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44013.543185636576</v>
       </c>
@@ -1742,7 +1760,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44013.568793171296</v>
       </c>
@@ -1942,7 +1960,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44013.584370335651</v>
       </c>
@@ -2142,7 +2160,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44013.612197847222</v>
       </c>
@@ -2333,7 +2351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44013.614569317127</v>
       </c>
@@ -2524,7 +2542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44013.647542569444</v>
       </c>
@@ -2724,7 +2742,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44013.674630856476</v>
       </c>
@@ -2915,7 +2933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44013.677036064815</v>
       </c>
@@ -3115,7 +3133,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44013.693406828708</v>
       </c>
@@ -3315,7 +3333,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44013.706331793983</v>
       </c>
@@ -3509,7 +3527,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44013.727114803245</v>
       </c>
@@ -3709,7 +3727,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44013.733918182872</v>
       </c>
@@ -3900,7 +3918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44013.738339722222</v>
       </c>
@@ -4100,7 +4118,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44013.744161400464</v>
       </c>
@@ -4300,7 +4318,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44013.762174409727</v>
       </c>
@@ -4500,7 +4518,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44013.764514618058</v>
       </c>
@@ -4700,7 +4718,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44013.777018379631</v>
       </c>
@@ -4891,7 +4909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44013.787945625001</v>
       </c>
@@ -5085,7 +5103,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44013.802506956017</v>
       </c>
@@ -5285,7 +5303,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44013.836942013892</v>
       </c>
@@ -5476,7 +5494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44013.853298553237</v>
       </c>
@@ -5670,7 +5688,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44013.886892858798</v>
       </c>
@@ -5861,7 +5879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44013.908742766202</v>
       </c>
@@ -6052,7 +6070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44014.542686493056</v>
       </c>
@@ -6252,7 +6270,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44014.648347951384</v>
       </c>
@@ -6443,7 +6461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44014.69049768518</v>
       </c>
@@ -6643,7 +6661,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44015.379597418985</v>
       </c>
@@ -6834,7 +6852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:66" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -6843,243 +6861,243 @@
         <v>23.466666666666665</v>
       </c>
       <c r="D32">
-        <f>SUM(D2:D31)/30</f>
+        <f t="shared" ref="D32:AI32" si="0">SUM(D2:D31)/30</f>
         <v>4.8666666666666663</v>
       </c>
       <c r="E32">
-        <f>SUM(E2:E31)/30</f>
+        <f t="shared" si="0"/>
         <v>6.0666666666666664</v>
       </c>
       <c r="F32">
-        <f>SUM(F2:F31)/30</f>
+        <f t="shared" si="0"/>
         <v>4.2333333333333334</v>
       </c>
       <c r="G32">
-        <f>SUM(G2:G31)/30</f>
+        <f t="shared" si="0"/>
         <v>7.666666666666667</v>
       </c>
       <c r="H32">
-        <f>SUM(H2:H31)/30</f>
+        <f t="shared" si="0"/>
         <v>6.8</v>
       </c>
       <c r="I32">
-        <f>SUM(I2:I31)/30</f>
+        <f t="shared" si="0"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="J32">
-        <f>SUM(J2:J31)/30</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K32">
-        <f>SUM(K2:K31)/30</f>
+        <f t="shared" si="0"/>
         <v>7.1333333333333337</v>
       </c>
       <c r="L32">
-        <f>SUM(L2:L31)/30</f>
+        <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
       <c r="M32">
-        <f>SUM(M2:M31)/30</f>
+        <f t="shared" si="0"/>
         <v>3.4333333333333331</v>
       </c>
       <c r="N32">
-        <f>SUM(N2:N31)/30</f>
+        <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
       <c r="O32">
-        <f>SUM(O2:O31)/30</f>
+        <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
       <c r="P32">
-        <f>SUM(P2:P31)/30</f>
+        <f t="shared" si="0"/>
         <v>3.1666666666666665</v>
       </c>
       <c r="Q32">
-        <f>SUM(Q2:Q31)/30</f>
+        <f t="shared" si="0"/>
         <v>7.166666666666667</v>
       </c>
       <c r="R32">
-        <f>SUM(R2:R31)/30</f>
+        <f t="shared" si="0"/>
         <v>5.0666666666666664</v>
       </c>
       <c r="S32">
-        <f>SUM(S2:S31)/30</f>
+        <f t="shared" si="0"/>
         <v>4.9333333333333336</v>
       </c>
       <c r="T32">
-        <f>SUM(T2:T31)/30</f>
+        <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
       <c r="U32">
-        <f>SUM(U2:U31)/30</f>
+        <f t="shared" si="0"/>
         <v>5.9</v>
       </c>
       <c r="V32">
-        <f>SUM(V2:V31)/30</f>
+        <f t="shared" si="0"/>
         <v>4.1333333333333337</v>
       </c>
       <c r="W32">
-        <f>SUM(W2:W31)/30</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="X32">
-        <f>SUM(X2:X31)/30</f>
+        <f t="shared" si="0"/>
         <v>6.5333333333333332</v>
       </c>
       <c r="Y32">
-        <f>SUM(Y2:Y31)/30</f>
+        <f t="shared" si="0"/>
         <v>6.1</v>
       </c>
       <c r="Z32">
-        <f>SUM(Z2:Z31)/30</f>
+        <f t="shared" si="0"/>
         <v>5.0666666666666664</v>
       </c>
       <c r="AA32">
-        <f>SUM(AA2:AA31)/30</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="AB32">
-        <f>SUM(AB2:AB31)/30</f>
+        <f t="shared" si="0"/>
         <v>5.8666666666666663</v>
       </c>
       <c r="AC32">
-        <f>SUM(AC2:AC31)/30</f>
+        <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
       <c r="AD32">
-        <f>SUM(AD2:AD31)/30</f>
+        <f t="shared" si="0"/>
         <v>4.9000000000000004</v>
       </c>
       <c r="AE32">
-        <f>SUM(AE2:AE31)/30</f>
+        <f t="shared" si="0"/>
         <v>1.5333333333333334</v>
       </c>
       <c r="AF32">
-        <f>SUM(AF2:AF31)/30</f>
+        <f t="shared" si="0"/>
         <v>7.5333333333333332</v>
       </c>
       <c r="AG32">
-        <f>SUM(AG2:AG31)/30</f>
+        <f t="shared" si="0"/>
         <v>3.1666666666666665</v>
       </c>
       <c r="AH32">
-        <f>SUM(AH2:AH31)/30</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="AI32">
-        <f>SUM(AI2:AI31)/30</f>
+        <f t="shared" si="0"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="AJ32">
-        <f>SUM(AJ2:AJ31)/30</f>
+        <f t="shared" ref="AJ32:BO32" si="1">SUM(AJ2:AJ31)/30</f>
         <v>1.6333333333333333</v>
       </c>
       <c r="AK32">
-        <f>SUM(AK2:AK31)/30</f>
+        <f t="shared" si="1"/>
         <v>7.8666666666666663</v>
       </c>
       <c r="AL32">
-        <f>SUM(AL2:AL31)/30</f>
+        <f t="shared" si="1"/>
         <v>6.0666666666666664</v>
       </c>
       <c r="AM32">
-        <f>SUM(AM2:AM31)/30</f>
+        <f t="shared" si="1"/>
         <v>7.8</v>
       </c>
       <c r="AN32">
-        <f>SUM(AN2:AN31)/30</f>
+        <f t="shared" si="1"/>
         <v>7.1333333333333337</v>
       </c>
       <c r="AO32">
-        <f>SUM(AO2:AO31)/30</f>
+        <f t="shared" si="1"/>
         <v>3.5666666666666669</v>
       </c>
       <c r="AP32">
-        <f>SUM(AP2:AP31)/30</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="AQ32">
-        <f>SUM(AQ2:AQ31)/30</f>
+        <f t="shared" si="1"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="AR32">
-        <f>SUM(AR2:AR31)/30</f>
+        <f t="shared" si="1"/>
         <v>0.56666666666666665</v>
       </c>
       <c r="AS32">
-        <f>SUM(AS2:AS31)/30</f>
+        <f t="shared" si="1"/>
         <v>2.9</v>
       </c>
       <c r="AT32">
-        <f>SUM(AT2:AT31)/30</f>
+        <f t="shared" si="1"/>
         <v>7.6333333333333337</v>
       </c>
       <c r="AU32">
-        <f>SUM(AU2:AU31)/30</f>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="AV32">
-        <f>SUM(AV2:AV31)/30</f>
+        <f t="shared" si="1"/>
         <v>7.9333333333333336</v>
       </c>
       <c r="AW32">
-        <f>SUM(AW2:AW31)/30</f>
+        <f t="shared" si="1"/>
         <v>1.8666666666666667</v>
       </c>
       <c r="AX32">
-        <f>SUM(AX2:AX31)/30</f>
+        <f t="shared" si="1"/>
         <v>5.166666666666667</v>
       </c>
       <c r="AY32">
-        <f>SUM(AY2:AY31)/30</f>
+        <f t="shared" si="1"/>
         <v>5.4666666666666668</v>
       </c>
       <c r="AZ32">
-        <f>SUM(AZ2:AZ31)/30</f>
+        <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
       <c r="BA32">
-        <f>SUM(BA2:BA31)/30</f>
+        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
       <c r="BB32">
-        <f>SUM(BB2:BB31)/30</f>
+        <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
       <c r="BC32">
-        <f>SUM(BC2:BC31)/30</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="BD32">
-        <f>SUM(BD2:BD31)/30</f>
+        <f t="shared" si="1"/>
         <v>5.7666666666666666</v>
       </c>
       <c r="BE32">
-        <f>SUM(BE2:BE31)/30</f>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
       <c r="BF32">
-        <f>SUM(BF2:BF31)/30</f>
+        <f t="shared" si="1"/>
         <v>3.5666666666666669</v>
       </c>
       <c r="BG32">
-        <f>SUM(BG2:BG31)/30</f>
+        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="BH32">
-        <f>SUM(BH2:BH31)/30</f>
+        <f t="shared" si="1"/>
         <v>5.0999999999999996</v>
       </c>
       <c r="BI32">
-        <f>SUM(BI2:BI31)/30</f>
+        <f t="shared" si="1"/>
         <v>5.2333333333333334</v>
       </c>
       <c r="BJ32">
-        <f>SUM(BJ2:BJ31)/30</f>
+        <f t="shared" si="1"/>
         <v>4.3666666666666663</v>
       </c>
       <c r="BK32">
-        <f>SUM(BK2:BK31)/30</f>
+        <f t="shared" si="1"/>
         <v>6.166666666666667</v>
       </c>
     </row>
@@ -7088,243 +7106,243 @@
         <v>117</v>
       </c>
       <c r="D33">
-        <f>STDEV(D2:D31)</f>
+        <f t="shared" ref="D33:AI33" si="2">STDEV(D2:D31)</f>
         <v>1.9605300714142442</v>
       </c>
       <c r="E33">
-        <f>STDEV(E2:E31)</f>
+        <f t="shared" si="2"/>
         <v>2.7907894487270863</v>
       </c>
       <c r="F33">
-        <f>STDEV(F2:F31)</f>
+        <f t="shared" si="2"/>
         <v>1.977168531587242</v>
       </c>
       <c r="G33">
-        <f>STDEV(G2:G31)</f>
+        <f t="shared" si="2"/>
         <v>2.1063669217862793</v>
       </c>
       <c r="H33">
-        <f>STDEV(H2:H31)</f>
+        <f t="shared" si="2"/>
         <v>2.3982752423212466</v>
       </c>
       <c r="I33">
-        <f>STDEV(I2:I31)</f>
+        <f t="shared" si="2"/>
         <v>2.0356026530046427</v>
       </c>
       <c r="J33">
-        <f>STDEV(J2:J31)</f>
+        <f t="shared" si="2"/>
         <v>2.5997347344787261</v>
       </c>
       <c r="K33">
-        <f>STDEV(K2:K31)</f>
+        <f t="shared" si="2"/>
         <v>2.1772068999195899</v>
       </c>
       <c r="L33">
-        <f>STDEV(L2:L31)</f>
+        <f t="shared" si="2"/>
         <v>1.7733661737517428</v>
       </c>
       <c r="M33">
-        <f>STDEV(M2:M31)</f>
+        <f t="shared" si="2"/>
         <v>2.2234383645425253</v>
       </c>
       <c r="N33">
-        <f>STDEV(N2:N31)</f>
+        <f t="shared" si="2"/>
         <v>1.323527157987713</v>
       </c>
       <c r="O33">
-        <f>STDEV(O2:O31)</f>
+        <f t="shared" si="2"/>
         <v>1.9722208731310475</v>
       </c>
       <c r="P33">
-        <f>STDEV(P2:P31)</f>
+        <f t="shared" si="2"/>
         <v>2.1827431860143225</v>
       </c>
       <c r="Q33">
-        <f>STDEV(Q2:Q31)</f>
+        <f t="shared" si="2"/>
         <v>1.510499650911016</v>
       </c>
       <c r="R33">
-        <f>STDEV(R2:R31)</f>
+        <f t="shared" si="2"/>
         <v>2.2273121784406165</v>
       </c>
       <c r="S33">
-        <f>STDEV(S2:S31)</f>
+        <f t="shared" si="2"/>
         <v>1.3113124074319811</v>
       </c>
       <c r="T33">
-        <f>STDEV(T2:T31)</f>
+        <f t="shared" si="2"/>
         <v>1.8067561584486038</v>
       </c>
       <c r="U33">
-        <f>STDEV(U2:U31)</f>
+        <f t="shared" si="2"/>
         <v>2.3540134473585383</v>
       </c>
       <c r="V33">
-        <f>STDEV(V2:V31)</f>
+        <f t="shared" si="2"/>
         <v>1.833281085984876</v>
       </c>
       <c r="W33">
-        <f>STDEV(W2:W31)</f>
+        <f t="shared" si="2"/>
         <v>2.0341905108624312</v>
       </c>
       <c r="X33">
-        <f>STDEV(X2:X31)</f>
+        <f t="shared" si="2"/>
         <v>2.3004247483863729</v>
       </c>
       <c r="Y33">
-        <f>STDEV(Y2:Y31)</f>
+        <f t="shared" si="2"/>
         <v>1.3222238320605808</v>
       </c>
       <c r="Z33">
-        <f>STDEV(Z2:Z31)</f>
+        <f t="shared" si="2"/>
         <v>2.3183426501874482</v>
       </c>
       <c r="AA33">
-        <f>STDEV(AA2:AA31)</f>
+        <f t="shared" si="2"/>
         <v>1.0938700673013826</v>
       </c>
       <c r="AB33">
-        <f>STDEV(AB2:AB31)</f>
+        <f t="shared" si="2"/>
         <v>3.1154048094006632</v>
       </c>
       <c r="AC33">
-        <f>STDEV(AC2:AC31)</f>
+        <f t="shared" si="2"/>
         <v>1.7498768429570237</v>
       </c>
       <c r="AD33">
-        <f>STDEV(AD2:AD31)</f>
+        <f t="shared" si="2"/>
         <v>2.294671488771173</v>
       </c>
       <c r="AE33">
-        <f>STDEV(AE2:AE31)</f>
+        <f t="shared" si="2"/>
         <v>1.6131642354623141</v>
       </c>
       <c r="AF33">
-        <f>STDEV(AF2:AF31)</f>
+        <f t="shared" si="2"/>
         <v>1.7759569219172373</v>
       </c>
       <c r="AG33">
-        <f>STDEV(AG2:AG31)</f>
+        <f t="shared" si="2"/>
         <v>1.9666764075348093</v>
       </c>
       <c r="AH33">
-        <f>STDEV(AH2:AH31)</f>
+        <f t="shared" si="2"/>
         <v>1.5624913792865636</v>
       </c>
       <c r="AI33">
-        <f>STDEV(AI2:AI31)</f>
+        <f t="shared" si="2"/>
         <v>1.6049492418657729</v>
       </c>
       <c r="AJ33">
-        <f>STDEV(AJ2:AJ31)</f>
+        <f t="shared" ref="AJ33:BK33" si="3">STDEV(AJ2:AJ31)</f>
         <v>2.2203344472108846</v>
       </c>
       <c r="AK33">
-        <f>STDEV(AK2:AK31)</f>
+        <f t="shared" si="3"/>
         <v>2.1129050655654065</v>
       </c>
       <c r="AL33">
-        <f>STDEV(AL2:AL31)</f>
+        <f t="shared" si="3"/>
         <v>2.8759805923921129</v>
       </c>
       <c r="AM33">
-        <f>STDEV(AM2:AM31)</f>
+        <f t="shared" si="3"/>
         <v>1.5844067746592745</v>
       </c>
       <c r="AN33">
-        <f>STDEV(AN2:AN31)</f>
+        <f t="shared" si="3"/>
         <v>1.8143742786394725</v>
       </c>
       <c r="AO33">
-        <f>STDEV(AO2:AO31)</f>
+        <f t="shared" si="3"/>
         <v>1.9061304607327731</v>
       </c>
       <c r="AP33">
-        <f>STDEV(AP2:AP31)</f>
+        <f t="shared" si="3"/>
         <v>3.0663168216240657</v>
       </c>
       <c r="AQ33">
-        <f>STDEV(AQ2:AQ31)</f>
+        <f t="shared" si="3"/>
         <v>2.0398332138265336</v>
       </c>
       <c r="AR33">
-        <f>STDEV(AR2:AR31)</f>
+        <f t="shared" si="3"/>
         <v>0.89763418297031317</v>
       </c>
       <c r="AS33">
-        <f>STDEV(AS2:AS31)</f>
+        <f t="shared" si="3"/>
         <v>1.8070742213255409</v>
       </c>
       <c r="AT33">
-        <f>STDEV(AT2:AT31)</f>
+        <f t="shared" si="3"/>
         <v>2.0254132542705241</v>
       </c>
       <c r="AU33">
-        <f>STDEV(AU2:AU31)</f>
+        <f t="shared" si="3"/>
         <v>2.0611346055192432</v>
       </c>
       <c r="AV33">
-        <f>STDEV(AV2:AV31)</f>
+        <f t="shared" si="3"/>
         <v>1.3628907749221184</v>
       </c>
       <c r="AW33">
-        <f>STDEV(AW2:AW31)</f>
+        <f t="shared" si="3"/>
         <v>2.1929877797878516</v>
       </c>
       <c r="AX33">
-        <f>STDEV(AX2:AX31)</f>
+        <f t="shared" si="3"/>
         <v>2.3937178316316361</v>
       </c>
       <c r="AY33">
-        <f>STDEV(AY2:AY31)</f>
+        <f t="shared" si="3"/>
         <v>2.5289132643984797</v>
       </c>
       <c r="AZ33">
-        <f>STDEV(AZ2:AZ31)</f>
+        <f t="shared" si="3"/>
         <v>2.2803508501982757</v>
       </c>
       <c r="BA33">
-        <f>STDEV(BA2:BA31)</f>
+        <f t="shared" si="3"/>
         <v>1.8146910062806456</v>
       </c>
       <c r="BB33">
-        <f>STDEV(BB2:BB31)</f>
+        <f t="shared" si="3"/>
         <v>1.8495106528950878</v>
       </c>
       <c r="BC33">
-        <f>STDEV(BC2:BC31)</f>
+        <f t="shared" si="3"/>
         <v>1.2410599844719297</v>
       </c>
       <c r="BD33">
-        <f>STDEV(BD2:BD31)</f>
+        <f t="shared" si="3"/>
         <v>2.6481396636433132</v>
       </c>
       <c r="BE33">
-        <f>STDEV(BE2:BE31)</f>
+        <f t="shared" si="3"/>
         <v>2.6490076216029173</v>
       </c>
       <c r="BF33">
-        <f>STDEV(BF2:BF31)</f>
+        <f t="shared" si="3"/>
         <v>1.8134237638032753</v>
       </c>
       <c r="BG33">
-        <f>STDEV(BG2:BG31)</f>
+        <f t="shared" si="3"/>
         <v>1.7086662137132156</v>
       </c>
       <c r="BH33">
-        <f>STDEV(BH2:BH31)</f>
+        <f t="shared" si="3"/>
         <v>2.7461571896642822</v>
       </c>
       <c r="BI33">
-        <f>STDEV(BI2:BI31)</f>
+        <f t="shared" si="3"/>
         <v>1.8323403789601473</v>
       </c>
       <c r="BJ33">
-        <f>STDEV(BJ2:BJ31)</f>
+        <f t="shared" si="3"/>
         <v>2.3116397126108432</v>
       </c>
       <c r="BK33">
-        <f>STDEV(BK2:BK31)</f>
+        <f t="shared" si="3"/>
         <v>2.1022702561481146</v>
       </c>
     </row>
@@ -7599,13 +7617,30 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="18:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R49" s="6"/>
       <c r="AL49" s="6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="18:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" t="s">
+        <v>138</v>
+      </c>
+      <c r="E50">
+        <f>AVERAGE(D33:W33)</f>
+        <v>2.029916784905224</v>
+      </c>
+      <c r="F50" t="s">
+        <v>141</v>
+      </c>
+      <c r="G50">
+        <f>AVERAGE(D33:H33,N33:R33)</f>
+        <v>2.0449433262320813</v>
+      </c>
       <c r="AB50" s="6" t="s">
         <v>131</v>
       </c>
@@ -7616,7 +7651,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="18:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>142</v>
+      </c>
+      <c r="G51">
+        <f>AVERAGE(I33:M33,S33:W33)</f>
+        <v>2.0148902435783658</v>
+      </c>
       <c r="AB51" s="6" t="s">
         <v>132</v>
       </c>
@@ -7625,6 +7667,56 @@
       </c>
       <c r="BG51" s="6" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="3:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52">
+        <f>AVERAGE(X33:AQ33)</f>
+        <v>2.0169167139890929</v>
+      </c>
+      <c r="F52" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52">
+        <f>AVERAGE(X33:AB33,AH33:AL33)</f>
+        <v>2.0526926833657191</v>
+      </c>
+    </row>
+    <row r="53" spans="3:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>142</v>
+      </c>
+      <c r="G53">
+        <f>AVERAGE(AC33:AG33,AM33:AQ33)</f>
+        <v>1.981140744612468</v>
+      </c>
+    </row>
+    <row r="54" spans="3:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54">
+        <f>AVERAGE(AR33:BK33)</f>
+        <v>2.0133511604408878</v>
+      </c>
+      <c r="F54" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54">
+        <f>AVERAGE(AR33:AV33,BB33:BF33)</f>
+        <v>1.8355288725424264</v>
+      </c>
+    </row>
+    <row r="55" spans="3:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>142</v>
+      </c>
+      <c r="G55">
+        <f>AVERAGE(BG33:BK33,AW33:BA33)</f>
+        <v>2.1911734483393492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>